<commit_message>
Nytt forsøk på oppdatering av ssbtabell 10484
</commit_message>
<xml_diff>
--- a/Data/05_Mobilitet og infrastruktur/SSB10484_Jernbanetransport.xlsx
+++ b/Data/05_Mobilitet og infrastruktur/SSB10484_Jernbanetransport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arbeidsområde\github\Telemark\Data\05_Mobilitet og infrastruktur\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://telemarkfylke-my.sharepoint.com/personal/kjell-tore_haustveit_telemarkfylke_no/Documents/GitHub/Telemark/Data/05_Mobilitet og infrastruktur/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85C5B52B-52F5-458B-9C0D-7528D974B293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D90020A2-4212-4A61-B1EE-589C0E8075B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="28776" windowHeight="16248" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25140" yWindow="384" windowWidth="22488" windowHeight="15696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Passasjerer" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>10484: Persontransport med jernbane, etter år, statistikkvariabel og togstrekning</t>
   </si>
@@ -71,13 +71,19 @@
     <t>2021</t>
   </si>
   <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
     <t>Sist endret:</t>
   </si>
   <si>
     <t>Passasjerer (påstigninger):</t>
   </si>
   <si>
-    <t>20220608 08:00</t>
+    <t>20240530 08:00</t>
   </si>
   <si>
     <t>Transportarbeid (passasjerkm):</t>
@@ -92,16 +98,13 @@
     <t>Kontakt:</t>
   </si>
   <si>
-    <t>Jan Sebastian Rothe, Statistisk sentralbyrå</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +47 91 31 99 06</t>
-  </si>
-  <si>
-    <t>jsr@ssb.no</t>
-  </si>
-  <si>
-    <t>Copyright</t>
+    <t>Jardar Andersen, Statistisk sentralbyrå</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +47 99700804</t>
+  </si>
+  <si>
+    <t>jrs@ssb.no</t>
   </si>
   <si>
     <t>Måleenhet:</t>
@@ -123,6 +126,9 @@
   </si>
   <si>
     <t>01.01-31.12</t>
+  </si>
+  <si>
+    <t>Offisiell statistikk</t>
   </si>
   <si>
     <t>Database:</t>
@@ -184,10 +190,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -645,14 +651,38 @@
         <v>98151109</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B12" s="3">
+        <v>7003721</v>
+      </c>
+      <c r="C12" s="3">
+        <v>680442</v>
+      </c>
+      <c r="D12" s="3">
+        <v>382863998</v>
+      </c>
+      <c r="E12" s="3">
+        <v>177893572</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="B13" s="3">
+        <v>8214088</v>
+      </c>
+      <c r="C13" s="3">
+        <v>744541</v>
+      </c>
+      <c r="D13" s="3">
+        <v>489976853</v>
+      </c>
+      <c r="E13" s="3">
+        <v>186400759</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -667,7 +697,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
@@ -675,29 +710,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>17</v>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
@@ -705,34 +735,34 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
@@ -742,67 +772,77 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>